<commit_message>
add script for MLST result per species
</commit_message>
<xml_diff>
--- a/data_files/04July2024_SampleSheet.xlsx
+++ b/data_files/04July2024_SampleSheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="140">
   <si>
     <t>[Header]</t>
   </si>
@@ -437,6 +437,9 @@
   </si>
   <si>
     <t>Estimated Yield</t>
+  </si>
+  <si>
+    <t>index reads</t>
   </si>
 </sst>
 </file>
@@ -1366,8 +1369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19:K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2190,15 +2193,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -2226,8 +2239,11 @@
       <c r="I1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -2255,8 +2271,11 @@
       <c r="I2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <v>4.2380000000000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -2284,8 +2303,11 @@
       <c r="I3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3">
+        <v>7.1864999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -2313,8 +2335,11 @@
       <c r="I4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <v>4.3914</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -2342,8 +2367,11 @@
       <c r="I5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <v>4.0486000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -2371,8 +2399,11 @@
       <c r="I6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <v>4.1349</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>63</v>
       </c>
@@ -2400,8 +2431,11 @@
       <c r="I7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <v>5.2478999999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>70</v>
       </c>
@@ -2429,8 +2463,11 @@
       <c r="I8" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <v>3.9510000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>77</v>
       </c>
@@ -2458,8 +2495,11 @@
       <c r="I9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9">
+        <v>3.4445999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>84</v>
       </c>
@@ -2487,8 +2527,11 @@
       <c r="I10" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <v>4.4531000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>89</v>
       </c>
@@ -2516,8 +2559,11 @@
       <c r="I11" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <v>4.8521999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>94</v>
       </c>
@@ -2545,8 +2591,11 @@
       <c r="I12" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <v>7.5054999999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>97</v>
       </c>
@@ -2574,8 +2623,11 @@
       <c r="I13" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13">
+        <v>6.9987000000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>102</v>
       </c>
@@ -2603,8 +2655,11 @@
       <c r="I14" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>105</v>
       </c>
@@ -2632,8 +2687,11 @@
       <c r="I15" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15">
+        <v>6.07</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>108</v>
       </c>
@@ -2661,8 +2719,11 @@
       <c r="I16" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16">
+        <v>4.4333999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>111</v>
       </c>
@@ -2690,8 +2751,11 @@
       <c r="I17" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17">
+        <v>5.8227000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>114</v>
       </c>
@@ -2719,8 +2783,11 @@
       <c r="I18" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18">
+        <v>4.0411999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>117</v>
       </c>
@@ -2748,8 +2815,11 @@
       <c r="I19" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19">
+        <v>3.7890000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>120</v>
       </c>
@@ -2777,8 +2847,11 @@
       <c r="I20" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20">
+        <v>2.2545000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>123</v>
       </c>
@@ -2806,8 +2879,11 @@
       <c r="I21" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21">
+        <v>4.3098999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>128</v>
       </c>
@@ -2835,8 +2911,11 @@
       <c r="I22" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22">
+        <v>2.7637</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>131</v>
       </c>
@@ -2863,6 +2942,9 @@
       </c>
       <c r="I23" t="s">
         <v>3</v>
+      </c>
+      <c r="J23">
+        <v>0.84289999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>